<commit_message>
Update and add results of new experiments
</commit_message>
<xml_diff>
--- a/results/catboost_categorical_processing/results_all_metrics.xlsx
+++ b/results/catboost_categorical_processing/results_all_metrics.xlsx
@@ -968,7 +968,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>f1 score</t>
+          <t>AUC</t>
         </is>
       </c>
     </row>
@@ -992,7 +992,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>f1 score</t>
+          <t>AUC</t>
         </is>
       </c>
     </row>
@@ -1007,7 +1007,7 @@
         <v>1</v>
       </c>
       <c r="D24" t="n">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1016,7 +1016,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>f1 score</t>
+          <t>AUC</t>
         </is>
       </c>
     </row>
@@ -1040,7 +1040,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>f1 score</t>
+          <t>AUC</t>
         </is>
       </c>
     </row>
@@ -1064,7 +1064,7 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>f1 score</t>
+          <t>AUC</t>
         </is>
       </c>
     </row>
@@ -1088,13 +1088,13 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>f1 score</t>
+          <t>AUC</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="B28" t="n">
         <v>1</v>
@@ -1112,7 +1112,7 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>f1 score</t>
+          <t>AUC</t>
         </is>
       </c>
     </row>
@@ -1124,7 +1124,7 @@
         <v>1</v>
       </c>
       <c r="C29" t="n">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="D29" t="n">
         <v>1</v>
@@ -1136,7 +1136,7 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>f1 score</t>
+          <t>AUC</t>
         </is>
       </c>
     </row>
@@ -1160,7 +1160,7 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>f1 score</t>
+          <t>AUC</t>
         </is>
       </c>
     </row>
@@ -1172,7 +1172,7 @@
         <v>1</v>
       </c>
       <c r="C31" t="n">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="D31" t="n">
         <v>1</v>
@@ -1184,22 +1184,22 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>f1 score</t>
+          <t>AUC</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>0.9701611616403383</v>
+        <v>0.817540847657428</v>
       </c>
       <c r="B32" t="n">
-        <v>0.9723057445798385</v>
+        <v>0.8669375565424788</v>
       </c>
       <c r="C32" t="n">
-        <v>0.9730329949238578</v>
+        <v>0.8685841420621214</v>
       </c>
       <c r="D32" t="n">
-        <v>0.9720158102766797</v>
+        <v>0.819241405543219</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -1208,22 +1208,22 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>f1 score</t>
+          <t>AUC</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>0.9731715106994571</v>
+        <v>0.8133627011541519</v>
       </c>
       <c r="B33" t="n">
-        <v>0.9726550079491255</v>
+        <v>0.8592597732817941</v>
       </c>
       <c r="C33" t="n">
-        <v>0.9724653827789272</v>
+        <v>0.8560514159607424</v>
       </c>
       <c r="D33" t="n">
-        <v>0.972887268114793</v>
+        <v>0.7988244304630315</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1232,22 +1232,22 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>f1 score</t>
+          <t>AUC</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>0.970452004472129</v>
+        <v>0.8038182190169301</v>
       </c>
       <c r="B34" t="n">
-        <v>0.9713108258044064</v>
+        <v>0.8257471911070192</v>
       </c>
       <c r="C34" t="n">
-        <v>0.9716188362137308</v>
+        <v>0.823181252450855</v>
       </c>
       <c r="D34" t="n">
-        <v>0.9733840304182509</v>
+        <v>0.7818466233611239</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1256,22 +1256,22 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>f1 score</t>
+          <t>AUC</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>0.9707434052757794</v>
+        <v>0.8444887729527901</v>
       </c>
       <c r="B35" t="n">
-        <v>0.9717908082408876</v>
+        <v>0.8573764342829864</v>
       </c>
       <c r="C35" t="n">
-        <v>0.9714919227114349</v>
+        <v>0.857986803744054</v>
       </c>
       <c r="D35" t="n">
-        <v>0.9729558753756128</v>
+        <v>0.8167058803471264</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1280,22 +1280,22 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>f1 score</t>
+          <t>AUC</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>0.970635173954676</v>
+        <v>0.8291195676265493</v>
       </c>
       <c r="B36" t="n">
-        <v>0.9711568938193343</v>
+        <v>0.8477094095783677</v>
       </c>
       <c r="C36" t="n">
-        <v>0.9710927573062262</v>
+        <v>0.8376928716348694</v>
       </c>
       <c r="D36" t="n">
-        <v>0.9726309128302484</v>
+        <v>0.8025915127955945</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1304,22 +1304,22 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>f1 score</t>
+          <t>AUC</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>0.9696097248880359</v>
+        <v>0.8252877090685897</v>
       </c>
       <c r="B37" t="n">
-        <v>0.9736675126903552</v>
+        <v>0.8528685659727551</v>
       </c>
       <c r="C37" t="n">
-        <v>0.9736172917991099</v>
+        <v>0.8505421717559205</v>
       </c>
       <c r="D37" t="n">
-        <v>0.9721518987341772</v>
+        <v>0.7917387004927284</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1328,22 +1328,22 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>f1 score</t>
+          <t>AUC</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>0.9691840970780776</v>
+        <v>0.8168218164458767</v>
       </c>
       <c r="B38" t="n">
-        <v>0.9724247226624406</v>
+        <v>0.8651023818048522</v>
       </c>
       <c r="C38" t="n">
-        <v>0.9739847715736041</v>
+        <v>0.8645568001636745</v>
       </c>
       <c r="D38" t="n">
-        <v>0.9739930225182365</v>
+        <v>0.7966165413533833</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -1352,22 +1352,22 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>f1 score</t>
+          <t>AUC</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>0.9699392388871122</v>
+        <v>0.8252237737200143</v>
       </c>
       <c r="B39" t="n">
-        <v>0.9726636999364272</v>
+        <v>0.8790104512983137</v>
       </c>
       <c r="C39" t="n">
-        <v>0.9714194982534137</v>
+        <v>0.870408163265306</v>
       </c>
       <c r="D39" t="n">
-        <v>0.9740341988600379</v>
+        <v>0.8421555589654408</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -1376,22 +1376,22 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>f1 score</t>
+          <t>AUC</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>0.9714468017227628</v>
+        <v>0.8666589944248376</v>
       </c>
       <c r="B40" t="n">
-        <v>0.9717549984132021</v>
+        <v>0.9025096755494176</v>
       </c>
       <c r="C40" t="n">
-        <v>0.9723320158102767</v>
+        <v>0.9041276661040356</v>
       </c>
       <c r="D40" t="n">
-        <v>0.9727589483687045</v>
+        <v>0.8331841508533239</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -1400,22 +1400,22 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>f1 score</t>
+          <t>AUC</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>0.9709172259507829</v>
+        <v>0.8581540956014555</v>
       </c>
       <c r="B41" t="n">
-        <v>0.9729987293519695</v>
+        <v>0.8866101744300643</v>
       </c>
       <c r="C41" t="n">
-        <v>0.9733079122974261</v>
+        <v>0.8877431042963924</v>
       </c>
       <c r="D41" t="n">
-        <v>0.9729558753756128</v>
+        <v>0.836809251289329</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1424,22 +1424,22 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>f1 score</t>
+          <t>AUC</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>1</v>
+        <v>-0.0007834746323563267</v>
       </c>
       <c r="B42" t="n">
-        <v>1</v>
+        <v>-0.0004371154131972546</v>
       </c>
       <c r="C42" t="n">
-        <v>1</v>
+        <v>-0.0006668655307575344</v>
       </c>
       <c r="D42" t="n">
-        <v>1</v>
+        <v>-0.0005400911875440716</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1448,22 +1448,22 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>AUC</t>
+          <t>log loss</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>1</v>
+        <v>-0.0003969153974189798</v>
       </c>
       <c r="B43" t="n">
-        <v>1</v>
+        <v>-0.0005101248051727581</v>
       </c>
       <c r="C43" t="n">
-        <v>1</v>
+        <v>-0.0005647992604142721</v>
       </c>
       <c r="D43" t="n">
-        <v>1</v>
+        <v>-0.0004734058803413595</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -1472,22 +1472,22 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>AUC</t>
+          <t>log loss</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>1</v>
+        <v>-0.0004345655301062264</v>
       </c>
       <c r="B44" t="n">
-        <v>1</v>
+        <v>-0.0004035605680481028</v>
       </c>
       <c r="C44" t="n">
-        <v>1</v>
+        <v>-0.0004542955031632838</v>
       </c>
       <c r="D44" t="n">
-        <v>0.9999999999999999</v>
+        <v>-0.0005357143434201267</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -1496,22 +1496,22 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>AUC</t>
+          <t>log loss</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>1</v>
+        <v>-0.0003590763276736444</v>
       </c>
       <c r="B45" t="n">
-        <v>1</v>
+        <v>-0.000413723710588281</v>
       </c>
       <c r="C45" t="n">
-        <v>1</v>
+        <v>-0.0007882571745751351</v>
       </c>
       <c r="D45" t="n">
-        <v>1</v>
+        <v>-0.0003858812574854307</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1520,22 +1520,22 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>AUC</t>
+          <t>log loss</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>1</v>
+        <v>-0.0004178049407673643</v>
       </c>
       <c r="B46" t="n">
-        <v>1</v>
+        <v>-0.0002982008263123635</v>
       </c>
       <c r="C46" t="n">
-        <v>1</v>
+        <v>-0.0009739946674781173</v>
       </c>
       <c r="D46" t="n">
-        <v>1</v>
+        <v>-0.0005694326350820679</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -1544,22 +1544,22 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>AUC</t>
+          <t>log loss</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>1</v>
+        <v>-0.0004703871533440037</v>
       </c>
       <c r="B47" t="n">
-        <v>1</v>
+        <v>-0.0003488519342311819</v>
       </c>
       <c r="C47" t="n">
-        <v>1</v>
+        <v>-0.0005928242316756746</v>
       </c>
       <c r="D47" t="n">
-        <v>1</v>
+        <v>-0.0005294177855590024</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -1568,22 +1568,22 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>AUC</t>
+          <t>log loss</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>0.9999999999999999</v>
+        <v>-0.0004079153759773753</v>
       </c>
       <c r="B48" t="n">
-        <v>1</v>
+        <v>-0.0004619052853879943</v>
       </c>
       <c r="C48" t="n">
-        <v>1</v>
+        <v>-0.0009003213654714627</v>
       </c>
       <c r="D48" t="n">
-        <v>1</v>
+        <v>-0.0004810170234429494</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -1592,22 +1592,22 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>AUC</t>
+          <t>log loss</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>1</v>
+        <v>-0.0003385158698051249</v>
       </c>
       <c r="B49" t="n">
-        <v>1</v>
+        <v>-0.0004109182066639176</v>
       </c>
       <c r="C49" t="n">
-        <v>0.9999999999999999</v>
+        <v>-0.0006547624827905523</v>
       </c>
       <c r="D49" t="n">
-        <v>1</v>
+        <v>-0.0004030655356759185</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -1616,22 +1616,22 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>AUC</t>
+          <t>log loss</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>1</v>
+        <v>-0.0007331929347144702</v>
       </c>
       <c r="B50" t="n">
-        <v>1</v>
+        <v>-0.0006867943468819407</v>
       </c>
       <c r="C50" t="n">
-        <v>1</v>
+        <v>-0.002052529142241044</v>
       </c>
       <c r="D50" t="n">
-        <v>1</v>
+        <v>-0.0009452307090967786</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -1640,22 +1640,22 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>AUC</t>
+          <t>log loss</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>1</v>
+        <v>-0.0006567374207898593</v>
       </c>
       <c r="B51" t="n">
-        <v>1</v>
+        <v>-0.0007775325125011385</v>
       </c>
       <c r="C51" t="n">
-        <v>0.9999999999999999</v>
+        <v>-0.001147144579002779</v>
       </c>
       <c r="D51" t="n">
-        <v>1</v>
+        <v>-0.0008937360224664204</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -1664,22 +1664,22 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>AUC</t>
+          <t>log loss</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>0.817540847657428</v>
+        <v>-0.2425772749262943</v>
       </c>
       <c r="B52" t="n">
-        <v>0.8669375565424788</v>
+        <v>-0.1560163855876009</v>
       </c>
       <c r="C52" t="n">
-        <v>0.8685841420621214</v>
+        <v>-0.1551385649568812</v>
       </c>
       <c r="D52" t="n">
-        <v>0.819241405543219</v>
+        <v>-0.1715481444733716</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1688,22 +1688,22 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>AUC</t>
+          <t>log loss</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>0.8133627011541519</v>
+        <v>-0.2559245721234976</v>
       </c>
       <c r="B53" t="n">
-        <v>0.8592597732817941</v>
+        <v>-0.1572683465618068</v>
       </c>
       <c r="C53" t="n">
-        <v>0.8560514159607424</v>
+        <v>-0.1576150138725978</v>
       </c>
       <c r="D53" t="n">
-        <v>0.7988244304630315</v>
+        <v>-0.1657465342226435</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1712,22 +1712,22 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>AUC</t>
+          <t>log loss</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>0.8038182190169301</v>
+        <v>-0.2632588875092604</v>
       </c>
       <c r="B54" t="n">
-        <v>0.8257471911070192</v>
+        <v>-0.1643754880401221</v>
       </c>
       <c r="C54" t="n">
-        <v>0.823181252450855</v>
+        <v>-0.1631212811610824</v>
       </c>
       <c r="D54" t="n">
-        <v>0.7818466233611239</v>
+        <v>-0.1747094658981536</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -1736,22 +1736,22 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>AUC</t>
+          <t>log loss</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>0.8444887729527901</v>
+        <v>-0.2250558635004151</v>
       </c>
       <c r="B55" t="n">
-        <v>0.8573764342829864</v>
+        <v>-0.1595197546985891</v>
       </c>
       <c r="C55" t="n">
-        <v>0.857986803744054</v>
+        <v>-0.1576410364645288</v>
       </c>
       <c r="D55" t="n">
-        <v>0.8167058803471264</v>
+        <v>-0.1675316150967985</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1760,22 +1760,22 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>AUC</t>
+          <t>log loss</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>0.8291195676265493</v>
+        <v>-0.2372810302393573</v>
       </c>
       <c r="B56" t="n">
-        <v>0.8477094095783677</v>
+        <v>-0.1657850097608822</v>
       </c>
       <c r="C56" t="n">
-        <v>0.8376928716348694</v>
+        <v>-0.1685943439614503</v>
       </c>
       <c r="D56" t="n">
-        <v>0.8025915127955945</v>
+        <v>-0.1706282029611253</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1784,22 +1784,22 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>AUC</t>
+          <t>log loss</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>0.8252877090685897</v>
+        <v>-0.2514967118505977</v>
       </c>
       <c r="B57" t="n">
-        <v>0.8528685659727551</v>
+        <v>-0.1577106252078742</v>
       </c>
       <c r="C57" t="n">
-        <v>0.8505421717559205</v>
+        <v>-0.1573033080164973</v>
       </c>
       <c r="D57" t="n">
-        <v>0.7917387004927284</v>
+        <v>-0.1728537395840315</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -1808,22 +1808,22 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>AUC</t>
+          <t>log loss</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>0.8168218164458767</v>
+        <v>-0.2447620765013136</v>
       </c>
       <c r="B58" t="n">
-        <v>0.8651023818048522</v>
+        <v>-0.1547499616141116</v>
       </c>
       <c r="C58" t="n">
-        <v>0.8645568001636745</v>
+        <v>-0.1542666551808109</v>
       </c>
       <c r="D58" t="n">
-        <v>0.7966165413533833</v>
+        <v>-0.1680923461020287</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1832,22 +1832,22 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>AUC</t>
+          <t>log loss</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>0.8252237737200143</v>
+        <v>-0.2377780352155519</v>
       </c>
       <c r="B59" t="n">
-        <v>0.8790104512983137</v>
+        <v>-0.1505491647602472</v>
       </c>
       <c r="C59" t="n">
-        <v>0.870408163265306</v>
+        <v>-0.1556256236738262</v>
       </c>
       <c r="D59" t="n">
-        <v>0.8421555589654408</v>
+        <v>-0.1646216239942101</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -1856,22 +1856,22 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>AUC</t>
+          <t>log loss</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>0.8666589944248376</v>
+        <v>-0.2062961421409688</v>
       </c>
       <c r="B60" t="n">
-        <v>0.9025096755494176</v>
+        <v>-0.1456687701409266</v>
       </c>
       <c r="C60" t="n">
-        <v>0.9041276661040356</v>
+        <v>-0.1449686015754659</v>
       </c>
       <c r="D60" t="n">
-        <v>0.8331841508533239</v>
+        <v>-0.1643484120901253</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -1880,22 +1880,22 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>AUC</t>
+          <t>log loss</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>0.8581540956014555</v>
+        <v>-0.2043559304208107</v>
       </c>
       <c r="B61" t="n">
-        <v>0.8866101744300643</v>
+        <v>-0.1496997405738351</v>
       </c>
       <c r="C61" t="n">
-        <v>0.8877431042963924</v>
+        <v>-0.1496944343718555</v>
       </c>
       <c r="D61" t="n">
-        <v>0.836809251289329</v>
+        <v>-0.1640823944256502</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -1904,7 +1904,7 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>AUC</t>
+          <t>log loss</t>
         </is>
       </c>
     </row>

</xml_diff>